<commit_message>
add gcc option in makefile
</commit_message>
<xml_diff>
--- a/calc/doc/UnitTestData.xlsx
+++ b/calc/doc/UnitTestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="11340" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="11340" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="validateInputFormula" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="96">
   <si>
     <t>[IN]formula</t>
     <phoneticPr fontId="1"/>
@@ -360,10 +360,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>array</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>sp</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -413,6 +409,62 @@
   </si>
   <si>
     <t>[IN]stack</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>stack[0]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>stack[1]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>stack</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>spTemp</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[IN]operator</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[OUT]arrayResult</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[OUT]arrayTempReuslt</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>+/</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>\0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>arrayTemp</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -904,63 +956,63 @@
         <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" t="s">
         <v>72</v>
       </c>
-      <c r="C11" t="s">
-        <v>73</v>
-      </c>
       <c r="D11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" t="s">
         <v>72</v>
       </c>
-      <c r="C12" t="s">
-        <v>73</v>
-      </c>
       <c r="D12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" t="s">
         <v>80</v>
-      </c>
-      <c r="D13" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" t="s">
         <v>72</v>
       </c>
-      <c r="C14" t="s">
-        <v>73</v>
-      </c>
       <c r="D14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1497,8 +1549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="A1:E2"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1508,7 +1560,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" t="s">
         <v>63</v>
@@ -1558,7 +1610,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" t="s">
         <v>63</v>
@@ -1599,25 +1651,78 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:D1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="13.625" style="2" customWidth="1"/>
+    <col min="2" max="3" width="15.375" customWidth="1"/>
+    <col min="4" max="4" width="18.375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="25.625" style="2" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="3:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" t="s">
+        <v>85</v>
+      </c>
       <c r="C1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1625,9 +1730,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
@@ -1636,10 +1739,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" t="s">
         <v>69</v>
-      </c>
-      <c r="B1" t="s">
-        <v>70</v>
       </c>
       <c r="C1" t="s">
         <v>65</v>
@@ -1670,39 +1773,45 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" t="s">
         <v>69</v>
       </c>
-      <c r="B1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>65</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2">
-        <v>12</v>
+        <v>12.5</v>
       </c>
       <c r="B2">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" t="s">
+        <v>11.5</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>11.5</v>
+      </c>
+      <c r="E2" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added a optionfile and editted a jenkinsfile
</commit_message>
<xml_diff>
--- a/calc/doc/UnitTestData.xlsx
+++ b/calc/doc/UnitTestData.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="95">
   <si>
     <t>[IN]formula</t>
     <phoneticPr fontId="1"/>
@@ -444,14 +444,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>[OUT]arrayTempReuslt</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>+/</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>\0</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -464,7 +456,11 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>/</t>
+    <t>*/</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/,*,</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1651,10 +1647,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1662,12 +1658,11 @@
     <col min="1" max="1" width="13.625" style="2" customWidth="1"/>
     <col min="2" max="3" width="15.375" customWidth="1"/>
     <col min="4" max="4" width="18.375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="25.625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B1" t="s">
         <v>85</v>
@@ -1678,31 +1673,25 @@
       <c r="D1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>87</v>
       </c>
@@ -1713,10 +1702,7 @@
         <v>88</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>